<commit_message>
Changed codes metadata Extraction for longer unformatted codes, quick scape from creating code
</commit_message>
<xml_diff>
--- a/config/items.xlsx
+++ b/config/items.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\barcode_printer-win32-x64-1.0.0\resources\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\barcodeUtils\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4366DDC0-705C-4A1C-A329-32E18C9CF66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Nombre</t>
   </si>
@@ -104,22 +105,40 @@
     <t>SI</t>
   </si>
   <si>
-    <t>WR007-Balanza</t>
-  </si>
-  <si>
-    <t>T015-Taper</t>
-  </si>
-  <si>
-    <t>WR007</t>
-  </si>
-  <si>
-    <t>T015</t>
+    <t xml:space="preserve">N305-DELINE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N1035-ASDFA </t>
+  </si>
+  <si>
+    <t>N1036-N1036 -n1027</t>
+  </si>
+  <si>
+    <t>N1037-ORGANIZADOR DE PLATO PARA LAVATORIO</t>
+  </si>
+  <si>
+    <t>N1038-TETERA DE ALUMINIO</t>
+  </si>
+  <si>
+    <t>N305</t>
+  </si>
+  <si>
+    <t>N1035</t>
+  </si>
+  <si>
+    <t>N1036</t>
+  </si>
+  <si>
+    <t>N1037</t>
+  </si>
+  <si>
+    <t>N1038</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -464,33 +483,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
-    <col min="3" max="4" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="36.6640625" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" customWidth="1"/>
-    <col min="11" max="11" width="38.33203125" customWidth="1"/>
-    <col min="12" max="12" width="5.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
-    <col min="17" max="17" width="18.5546875" customWidth="1"/>
-    <col min="19" max="19" width="16.5546875" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="38.28515625" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -552,12 +571,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -566,7 +585,7 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -587,15 +606,15 @@
         <v>23</v>
       </c>
       <c r="T2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
@@ -604,7 +623,7 @@
         <v>21</v>
       </c>
       <c r="G3">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -625,7 +644,121 @@
         <v>24</v>
       </c>
       <c r="T3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dumb fix changed break in locator loop
</commit_message>
<xml_diff>
--- a/config/items.xlsx
+++ b/config/items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\barcodeUtils\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4366DDC0-705C-4A1C-A329-32E18C9CF66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7664546F-05CB-46DE-9D7B-6CBDE90AA928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Nombre</t>
   </si>
@@ -105,34 +105,10 @@
     <t>SI</t>
   </si>
   <si>
-    <t xml:space="preserve">N305-DELINE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N1035-ASDFA </t>
-  </si>
-  <si>
-    <t>N1036-N1036 -n1027</t>
-  </si>
-  <si>
-    <t>N1037-ORGANIZADOR DE PLATO PARA LAVATORIO</t>
-  </si>
-  <si>
-    <t>N1038-TETERA DE ALUMINIO</t>
-  </si>
-  <si>
     <t>N305</t>
   </si>
   <si>
-    <t>N1035</t>
-  </si>
-  <si>
-    <t>N1036</t>
-  </si>
-  <si>
-    <t>N1037</t>
-  </si>
-  <si>
-    <t>N1038</t>
+    <t>N305-EXPRIMIDOR DE NARANJA MANUAL</t>
   </si>
 </sst>
 </file>
@@ -485,7 +461,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -573,10 +549,10 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -585,7 +561,7 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -603,162 +579,10 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" t="s">
         <v>23</v>
-      </c>
-      <c r="T2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3">
-        <v>67</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3">
-        <v>10</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="P3" t="s">
-        <v>24</v>
-      </c>
-      <c r="T3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4">
-        <v>8</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4">
-        <v>10</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="P4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5">
-        <v>8</v>
-      </c>
-      <c r="H5">
-        <v>10</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5">
-        <v>10</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6">
-        <v>10</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="P6" t="s">
-        <v>27</v>
-      </c>
-      <c r="T6" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>